<commit_message>
adding shadowplayer to end turn message
</commit_message>
<xml_diff>
--- a/doc/Work.xlsx
+++ b/doc/Work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\desktop\Final Year\SoftwareEng\caffeine\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD7F3C8-8DF7-429A-896D-F80CF8CB55F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A4945B-3370-4714-BB6A-5B799B56771A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="117">
   <si>
     <t>Item</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>Refactored messaging interface to send shadowplayers in all requests.</t>
+  </si>
+  <si>
+    <t>Added.</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -739,8 +741,8 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,13 +782,13 @@
       <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>43378</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>43381</v>
       </c>
       <c r="F2" t="s">
@@ -800,13 +802,13 @@
       <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>43381</v>
       </c>
       <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>43390</v>
       </c>
       <c r="F3" t="s">
@@ -820,13 +822,13 @@
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -840,13 +842,13 @@
       <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>43381</v>
       </c>
       <c r="D5" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>43385</v>
       </c>
       <c r="F5" t="s">
@@ -860,13 +862,13 @@
       <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>43381</v>
       </c>
       <c r="D6" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>43385</v>
       </c>
       <c r="F6" t="s">
@@ -880,13 +882,13 @@
       <c r="B7" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>43386</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>43390</v>
       </c>
       <c r="F7" t="s">
@@ -900,13 +902,13 @@
       <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>43390</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>43405</v>
       </c>
       <c r="F8" t="s">
@@ -920,13 +922,13 @@
       <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>43390</v>
       </c>
       <c r="D9" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>43396</v>
       </c>
       <c r="F9" t="s">
@@ -940,13 +942,13 @@
       <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>43396</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>43401</v>
       </c>
       <c r="F10" t="s">
@@ -960,13 +962,13 @@
       <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>43396</v>
       </c>
       <c r="D11" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -975,13 +977,13 @@
       <c r="B12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>43397</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>43400</v>
       </c>
       <c r="F12" t="s">
@@ -995,13 +997,13 @@
       <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>43400</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>43400</v>
       </c>
       <c r="F13" t="s">
@@ -1015,13 +1017,13 @@
       <c r="B14" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>43400</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>43415</v>
       </c>
       <c r="F14" t="s">
@@ -1035,13 +1037,13 @@
       <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>43400</v>
       </c>
       <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>43415</v>
       </c>
       <c r="F15" t="s">
@@ -1055,13 +1057,13 @@
       <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>43400</v>
       </c>
       <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F16" t="s">
@@ -1075,13 +1077,13 @@
       <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>43400</v>
       </c>
       <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>43403</v>
       </c>
       <c r="F17" t="s">
@@ -1095,13 +1097,13 @@
       <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>43400</v>
       </c>
       <c r="D18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>43402</v>
       </c>
       <c r="F18" t="s">
@@ -1115,13 +1117,13 @@
       <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>43400</v>
       </c>
       <c r="D19" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>43403</v>
       </c>
       <c r="F19" t="s">
@@ -1135,13 +1137,13 @@
       <c r="B20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>43400</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>43411</v>
       </c>
       <c r="F20" t="s">
@@ -1155,13 +1157,13 @@
       <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>43400</v>
       </c>
       <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>43415</v>
       </c>
       <c r="F21" t="s">
@@ -1175,13 +1177,13 @@
       <c r="B22" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>43401</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>43401</v>
       </c>
       <c r="F22" t="s">
@@ -1195,13 +1197,13 @@
       <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>43401</v>
       </c>
       <c r="D23" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>43403</v>
       </c>
       <c r="F23" t="s">
@@ -1215,13 +1217,13 @@
       <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>43401</v>
       </c>
       <c r="D24" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>43425</v>
       </c>
       <c r="F24" t="s">
@@ -1235,13 +1237,13 @@
       <c r="B25" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>43401</v>
       </c>
       <c r="D25" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>43413</v>
       </c>
       <c r="F25" t="s">
@@ -1255,13 +1257,13 @@
       <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>43403</v>
       </c>
       <c r="D26" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>43403</v>
       </c>
       <c r="F26" t="s">
@@ -1275,13 +1277,13 @@
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>43403</v>
       </c>
       <c r="D27" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>43403</v>
       </c>
       <c r="F27" t="s">
@@ -1295,13 +1297,13 @@
       <c r="B28" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>43406</v>
       </c>
       <c r="D28" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>43408</v>
       </c>
       <c r="F28" t="s">
@@ -1315,7 +1317,7 @@
       <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>43409</v>
       </c>
       <c r="D29" t="s">
@@ -1332,13 +1334,13 @@
       <c r="B30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>43410</v>
       </c>
       <c r="D30" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>43412</v>
       </c>
       <c r="F30" t="s">
@@ -1352,13 +1354,13 @@
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>43410</v>
       </c>
       <c r="D31" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>43410</v>
       </c>
       <c r="F31" t="s">
@@ -1372,13 +1374,13 @@
       <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>43410</v>
       </c>
       <c r="D32" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>43412</v>
       </c>
       <c r="F32" t="s">
@@ -1392,13 +1394,13 @@
       <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>43410</v>
       </c>
       <c r="D33" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>43416</v>
       </c>
       <c r="F33" t="s">
@@ -1412,13 +1414,13 @@
       <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>43410</v>
       </c>
       <c r="D34" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>43425</v>
       </c>
       <c r="F34" t="s">
@@ -1432,13 +1434,13 @@
       <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>43410</v>
       </c>
       <c r="D35" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>43412</v>
       </c>
       <c r="F35" t="s">
@@ -1452,13 +1454,13 @@
       <c r="B36" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>43411</v>
       </c>
       <c r="D36" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>43435</v>
       </c>
       <c r="F36" t="s">
@@ -1472,13 +1474,13 @@
       <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>43411</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>43412</v>
       </c>
       <c r="F37" t="s">
@@ -1492,13 +1494,13 @@
       <c r="B38" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>43412</v>
       </c>
       <c r="D38" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>43412</v>
       </c>
       <c r="F38" t="s">
@@ -1523,13 +1525,13 @@
       <c r="B40" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>43412</v>
       </c>
       <c r="D40" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>43420</v>
       </c>
       <c r="F40" t="s">
@@ -1543,13 +1545,13 @@
       <c r="B41" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>43412</v>
       </c>
       <c r="D41" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>43412</v>
       </c>
       <c r="F41" t="s">
@@ -1563,13 +1565,13 @@
       <c r="B42" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>43412</v>
       </c>
       <c r="D42" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>43412</v>
       </c>
       <c r="F42" t="s">
@@ -1583,13 +1585,13 @@
       <c r="B43" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>43412</v>
       </c>
       <c r="D43" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>43415</v>
       </c>
       <c r="F43" t="s">
@@ -1603,13 +1605,13 @@
       <c r="B44" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>43412</v>
       </c>
       <c r="D44" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>43416</v>
       </c>
       <c r="F44" t="s">
@@ -1623,13 +1625,13 @@
       <c r="B45" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>43413</v>
       </c>
       <c r="D45" t="s">
         <v>74</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>43416</v>
       </c>
       <c r="F45" t="s">
@@ -1643,7 +1645,7 @@
       <c r="B46" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>43413</v>
       </c>
       <c r="D46" t="s">
@@ -1657,7 +1659,7 @@
       <c r="B47" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>43413</v>
       </c>
       <c r="D47" t="s">
@@ -1671,13 +1673,13 @@
       <c r="B48" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>43414</v>
       </c>
       <c r="D48" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>43415</v>
       </c>
       <c r="F48" t="s">
@@ -1691,13 +1693,13 @@
       <c r="B49" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>43414</v>
       </c>
       <c r="D49" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>43415</v>
       </c>
       <c r="F49" t="s">
@@ -1711,13 +1713,13 @@
       <c r="B50" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>43414</v>
       </c>
       <c r="D50" t="s">
         <v>71</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>43415</v>
       </c>
       <c r="F50" t="s">
@@ -1731,13 +1733,13 @@
       <c r="B51" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>43414</v>
       </c>
       <c r="D51" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>43415</v>
       </c>
       <c r="F51" t="s">
@@ -1751,13 +1753,13 @@
       <c r="B52" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>43419</v>
       </c>
       <c r="D52" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>43420</v>
       </c>
       <c r="F52" t="s">
@@ -1771,13 +1773,13 @@
       <c r="B53" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <v>43419</v>
       </c>
       <c r="D53" t="s">
         <v>71</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>43435</v>
       </c>
       <c r="F53" t="s">
@@ -1791,13 +1793,13 @@
       <c r="B54" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <v>43419</v>
       </c>
       <c r="D54" t="s">
         <v>70</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="2">
         <v>43435</v>
       </c>
       <c r="F54" t="s">
@@ -1811,7 +1813,7 @@
       <c r="B55" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <v>43420</v>
       </c>
       <c r="D55" t="s">
@@ -1825,13 +1827,13 @@
       <c r="B56" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <v>43429</v>
       </c>
       <c r="D56" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="2">
         <v>43433</v>
       </c>
       <c r="F56" t="s">
@@ -1845,7 +1847,7 @@
       <c r="B57" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="2">
         <v>43434</v>
       </c>
       <c r="D57" t="s">
@@ -1864,6 +1866,12 @@
       </c>
       <c r="D58" t="s">
         <v>70</v>
+      </c>
+      <c r="E58" s="2">
+        <v>43446</v>
+      </c>
+      <c r="F58" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added everything I could find
</commit_message>
<xml_diff>
--- a/doc/Work.xlsx
+++ b/doc/Work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\desktop\Final Year\SoftwareEng\caffeine\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A4945B-3370-4714-BB6A-5B799B56771A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E292B4DC-AA69-4816-8E77-AFD82248FC3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="162">
   <si>
     <t>Item</t>
   </si>
@@ -180,9 +180,6 @@
     <t xml:space="preserve">Are retired players immune </t>
   </si>
   <si>
-    <t>Ability to check if cards have been readded correctly to the deck</t>
-  </si>
-  <si>
     <t>Ability to return sold cards to deck</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>Decided the "bank" would manage this.</t>
   </si>
   <si>
-    <t>****</t>
-  </si>
-  <si>
     <t>Refactored existing code to implement this and used it going forwards where appropriate</t>
   </si>
   <si>
@@ -342,9 +336,6 @@
     <t>Cards now readded to the rear of the deck using existing but unused methods</t>
   </si>
   <si>
-    <t>***</t>
-  </si>
-  <si>
     <t>Unit tests created</t>
   </si>
   <si>
@@ -382,6 +373,150 @@
   </si>
   <si>
     <t>Added.</t>
+  </si>
+  <si>
+    <t>Spinner</t>
+  </si>
+  <si>
+    <t>Action Cards</t>
+  </si>
+  <si>
+    <t>House Cards</t>
+  </si>
+  <si>
+    <t>Career Cards</t>
+  </si>
+  <si>
+    <t>College Career Cards</t>
+  </si>
+  <si>
+    <t>Board (logic)</t>
+  </si>
+  <si>
+    <t>Payday Spaces</t>
+  </si>
+  <si>
+    <t>Action Spaces</t>
+  </si>
+  <si>
+    <t>Holiday Spaces</t>
+  </si>
+  <si>
+    <t>Spin to Win Spaces</t>
+  </si>
+  <si>
+    <t>Baby Spaces</t>
+  </si>
+  <si>
+    <t>House Spaces</t>
+  </si>
+  <si>
+    <t>Baby Stop</t>
+  </si>
+  <si>
+    <t>Core Feature</t>
+  </si>
+  <si>
+    <t>UI (basic)</t>
+  </si>
+  <si>
+    <t>UI board</t>
+  </si>
+  <si>
+    <t>UI input</t>
+  </si>
+  <si>
+    <t>"Bank"</t>
+  </si>
+  <si>
+    <t>UI data display</t>
+  </si>
+  <si>
+    <t>Maven</t>
+  </si>
+  <si>
+    <t>Config imports from json</t>
+  </si>
+  <si>
+    <t>Implemented using V,E graph to define edges and vertices.</t>
+  </si>
+  <si>
+    <t>Stored in JSON, read in and instances created via a factory.</t>
+  </si>
+  <si>
+    <t>"Player" Object</t>
+  </si>
+  <si>
+    <t>Created this object and defined the basic class variables.</t>
+  </si>
+  <si>
+    <t>Created a basic UI that will allow us to test the functionality going forward</t>
+  </si>
+  <si>
+    <t>Displays the relevant fields stored in the player object to the user</t>
+  </si>
+  <si>
+    <t>Allows for extensibility.</t>
+  </si>
+  <si>
+    <t>Taking out loans</t>
+  </si>
+  <si>
+    <t>Bank has responsibility for all monetary transactions.</t>
+  </si>
+  <si>
+    <t>Dependants</t>
+  </si>
+  <si>
+    <t>Marital status and dependants implemented.</t>
+  </si>
+  <si>
+    <t>Implemented the board, uses the same configuration file as the VE graph logical board.</t>
+  </si>
+  <si>
+    <t>Config file for resources and "magic" numbers</t>
+  </si>
+  <si>
+    <t>Implement "ShadowPlayer"  as a generic messaging object, rather than impl. Specific player</t>
+  </si>
+  <si>
+    <t>Button action listeners send messages to the logic and wait for a response.</t>
+  </si>
+  <si>
+    <t>Feature REquest</t>
+  </si>
+  <si>
+    <t>UI user decision</t>
+  </si>
+  <si>
+    <t>Binary choice for cards implemented.</t>
+  </si>
+  <si>
+    <t>Generates a random number from 1-10</t>
+  </si>
+  <si>
+    <t>Implemented as a separate state.</t>
+  </si>
+  <si>
+    <t>Forced in all cases apart from house purchase as otherwise it will force bankruptcy</t>
+  </si>
+  <si>
+    <t>Family Stop</t>
+  </si>
+  <si>
+    <t>Night School Stop</t>
+  </si>
+  <si>
+    <t>Graduation Stop</t>
+  </si>
+  <si>
+    <t>Get Married Stop</t>
+  </si>
+  <si>
+    <t>Retirement Stop</t>
+  </si>
+  <si>
+    <t>Was actually already done.</t>
   </si>
 </sst>
 </file>
@@ -738,16 +873,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021C5E94-141C-4B62-B501-75972CDFF5D4}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -780,1112 +915,1699 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2">
         <v>43378</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2">
         <v>43381</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2">
-        <v>43381</v>
+        <v>43378</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2">
-        <v>43390</v>
+        <v>43388</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>80</v>
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43378</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="2">
+        <v>43379</v>
+      </c>
+      <c r="F4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C5" s="2">
-        <v>43381</v>
+        <v>43378</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2">
-        <v>43385</v>
+        <v>43379</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C6" s="2">
-        <v>43381</v>
+        <v>43378</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2">
-        <v>43385</v>
+        <v>43380</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C7" s="2">
-        <v>43386</v>
+        <v>43378</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E7" s="2">
-        <v>43390</v>
+        <v>43380</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2">
-        <v>43390</v>
+        <v>43378</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E8" s="2">
-        <v>43405</v>
+        <v>43380</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C9" s="2">
-        <v>43390</v>
+        <v>43378</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2">
-        <v>43396</v>
+        <v>43391</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2">
-        <v>43396</v>
+        <v>43378</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="2">
-        <v>43401</v>
+        <v>43398</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2">
-        <v>43396</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>43378</v>
+      </c>
+      <c r="E11" s="2">
+        <v>43391</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C12" s="2">
-        <v>43397</v>
+        <v>43378</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2">
-        <v>43400</v>
+        <v>43398</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C13" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2">
         <v>43400</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C14" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2">
-        <v>43415</v>
+        <v>43397</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="C15" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E15" s="2">
-        <v>43415</v>
+        <v>43401</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="C16" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
+      </c>
+      <c r="E16" s="2">
+        <v>43398</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="C17" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E17" s="2">
-        <v>43403</v>
+        <v>43398</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C18" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E18" s="2">
-        <v>43402</v>
+        <v>43401</v>
       </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="C19" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="2">
-        <v>43403</v>
+        <v>43401</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="C20" s="2">
+        <v>43378</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="2">
         <v>43400</v>
       </c>
-      <c r="D20" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="2">
-        <v>43411</v>
-      </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C21" s="2">
-        <v>43400</v>
+        <v>43378</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E21" s="2">
-        <v>43415</v>
+        <v>43401</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="C22" s="2">
-        <v>43401</v>
+        <v>43378</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2">
-        <v>43401</v>
+        <v>43381</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="C23" s="2">
-        <v>43401</v>
+        <v>43378</v>
       </c>
       <c r="D23" t="s">
         <v>70</v>
       </c>
       <c r="E23" s="2">
-        <v>43403</v>
+        <v>43380</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="C24" s="2">
-        <v>43401</v>
+        <v>43378</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E24" s="2">
-        <v>43425</v>
+        <v>43381</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="C25" s="2">
-        <v>43401</v>
+        <v>43378</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E25" s="2">
-        <v>43413</v>
+        <v>43379</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="C26" s="2">
-        <v>43403</v>
+        <v>43378</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="2">
-        <v>43403</v>
+        <v>43446</v>
       </c>
       <c r="F26" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="C27" s="2">
-        <v>43403</v>
+        <v>43378</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="2">
-        <v>43403</v>
+        <v>43385</v>
       </c>
       <c r="F27" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="C28" s="2">
-        <v>43406</v>
+        <v>43378</v>
       </c>
       <c r="D28" t="s">
         <v>70</v>
       </c>
       <c r="E28" s="2">
-        <v>43408</v>
+        <v>43386</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="C29" s="2">
-        <v>43409</v>
+        <v>43378</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="E29" s="2">
+        <v>43381</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="C30" s="2">
-        <v>43410</v>
+        <v>43378</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30" s="2">
-        <v>43412</v>
+        <v>43379</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2">
-        <v>43410</v>
+        <v>43379</v>
       </c>
       <c r="D31" t="s">
         <v>70</v>
       </c>
       <c r="E31" s="2">
-        <v>43410</v>
+        <v>43379</v>
       </c>
       <c r="F31" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2">
-        <v>43410</v>
+        <v>43381</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="2">
-        <v>43412</v>
+        <v>43390</v>
       </c>
       <c r="F32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="C33" s="2">
-        <v>43410</v>
+        <v>43381</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="2">
-        <v>43416</v>
-      </c>
-      <c r="F33" t="s">
-        <v>96</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C34" s="2">
-        <v>43410</v>
+        <v>43381</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E34" s="2">
-        <v>43425</v>
+        <v>43385</v>
       </c>
       <c r="F34" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C35" s="2">
-        <v>43410</v>
+        <v>43381</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E35" s="2">
-        <v>43412</v>
+        <v>43385</v>
       </c>
       <c r="F35" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="C36" s="2">
-        <v>43411</v>
+        <v>43384</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E36" s="2">
-        <v>43435</v>
+        <v>43385</v>
       </c>
       <c r="F36" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C37" s="2">
-        <v>43411</v>
+        <v>43386</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E37" s="2">
-        <v>43412</v>
+        <v>43390</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" s="2">
-        <v>43412</v>
+        <v>43390</v>
       </c>
       <c r="D38" t="s">
         <v>70</v>
       </c>
       <c r="E38" s="2">
-        <v>43412</v>
+        <v>43405</v>
       </c>
       <c r="F38" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" t="s">
-        <v>103</v>
+        <v>57</v>
+      </c>
+      <c r="C39" s="2">
+        <v>43390</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="2">
+        <v>43396</v>
+      </c>
+      <c r="F39" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C40" s="2">
-        <v>43412</v>
+        <v>43396</v>
       </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E40" s="2">
-        <v>43420</v>
+        <v>43401</v>
       </c>
       <c r="F40" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
       <c r="C41" s="2">
-        <v>43412</v>
+        <v>43396</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="2">
-        <v>43412</v>
-      </c>
-      <c r="F41" t="s">
-        <v>105</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C42" s="2">
-        <v>43412</v>
+        <v>43397</v>
       </c>
       <c r="D42" t="s">
         <v>70</v>
       </c>
       <c r="E42" s="2">
-        <v>43412</v>
+        <v>43400</v>
       </c>
       <c r="F42" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="2">
-        <v>43412</v>
+        <v>43400</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E43" s="2">
-        <v>43415</v>
+        <v>43400</v>
       </c>
       <c r="F43" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C44" s="2">
-        <v>43412</v>
+        <v>43400</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E44" s="2">
-        <v>43416</v>
+        <v>43415</v>
       </c>
       <c r="F44" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
         <v>62</v>
       </c>
       <c r="C45" s="2">
-        <v>43413</v>
+        <v>43400</v>
       </c>
       <c r="D45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E45" s="2">
-        <v>43416</v>
+        <v>43415</v>
       </c>
       <c r="F45" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C46" s="2">
-        <v>43413</v>
+        <v>43400</v>
       </c>
       <c r="D46" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F46" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="2">
-        <v>43413</v>
+        <v>43400</v>
       </c>
       <c r="D47" t="s">
         <v>70</v>
       </c>
+      <c r="E47" s="2">
+        <v>43403</v>
+      </c>
+      <c r="F47" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C48" s="2">
-        <v>43414</v>
+        <v>43400</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E48" s="2">
-        <v>43415</v>
+        <v>43402</v>
       </c>
       <c r="F48" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C49" s="2">
-        <v>43414</v>
+        <v>43400</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E49" s="2">
-        <v>43415</v>
+        <v>43403</v>
       </c>
       <c r="F49" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C50" s="2">
-        <v>43414</v>
+        <v>43400</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E50" s="2">
-        <v>43415</v>
+        <v>43411</v>
       </c>
       <c r="F50" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2">
-        <v>43414</v>
+        <v>43400</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E51" s="2">
         <v>43415</v>
       </c>
       <c r="F51" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="2">
-        <v>43419</v>
+        <v>43401</v>
       </c>
       <c r="D52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E52" s="2">
-        <v>43420</v>
+        <v>43401</v>
       </c>
       <c r="F52" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C53" s="2">
-        <v>43419</v>
+        <v>43401</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E53" s="2">
-        <v>43435</v>
+        <v>43403</v>
       </c>
       <c r="F53" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C54" s="2">
-        <v>43419</v>
+        <v>43401</v>
       </c>
       <c r="D54" t="s">
         <v>70</v>
       </c>
       <c r="E54" s="2">
-        <v>43435</v>
+        <v>43425</v>
       </c>
       <c r="F54" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
         <v>63</v>
       </c>
       <c r="C55" s="2">
-        <v>43420</v>
+        <v>43401</v>
       </c>
       <c r="D55" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="E55" s="2">
+        <v>43413</v>
+      </c>
+      <c r="F55" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C56" s="2">
-        <v>43429</v>
+        <v>43403</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E56" s="2">
-        <v>43433</v>
+        <v>43403</v>
       </c>
       <c r="F56" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="2">
-        <v>43434</v>
+        <v>43403</v>
       </c>
       <c r="D57" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="E57" s="2">
+        <v>43403</v>
+      </c>
+      <c r="F57" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58" s="2">
-        <v>43446</v>
+        <v>43406</v>
       </c>
       <c r="D58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E58" s="2">
-        <v>43446</v>
+        <v>43408</v>
       </c>
       <c r="F58" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C59" s="2">
-        <v>43446</v>
+        <v>43409</v>
       </c>
       <c r="D59" t="s">
         <v>70</v>
+      </c>
+      <c r="F59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D61" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" s="2">
+        <v>43410</v>
+      </c>
+      <c r="F61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D62" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D63" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="2">
+        <v>43416</v>
+      </c>
+      <c r="F63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" s="2">
+        <v>43425</v>
+      </c>
+      <c r="F64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="2">
+        <v>43410</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="2">
+        <v>43411</v>
+      </c>
+      <c r="D66" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="2">
+        <v>43435</v>
+      </c>
+      <c r="F66" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="2">
+        <v>43411</v>
+      </c>
+      <c r="D67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B68" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" s="2">
+        <v>43412</v>
+      </c>
+      <c r="D68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="2">
+        <v>43412</v>
+      </c>
+      <c r="D69" t="s">
+        <v>73</v>
+      </c>
+      <c r="E69" s="2">
+        <v>43420</v>
+      </c>
+      <c r="F69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="2">
+        <v>43412</v>
+      </c>
+      <c r="D70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="2">
+        <v>43412</v>
+      </c>
+      <c r="D71" t="s">
+        <v>69</v>
+      </c>
+      <c r="E71" s="2">
+        <v>43412</v>
+      </c>
+      <c r="F71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" t="s">
+        <v>57</v>
+      </c>
+      <c r="C72" s="2">
+        <v>43412</v>
+      </c>
+      <c r="D72" t="s">
+        <v>69</v>
+      </c>
+      <c r="E72" s="2">
+        <v>43415</v>
+      </c>
+      <c r="F72" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="2">
+        <v>43412</v>
+      </c>
+      <c r="D73" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" s="2">
+        <v>43416</v>
+      </c>
+      <c r="F73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="2">
+        <v>43413</v>
+      </c>
+      <c r="D74" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" s="2">
+        <v>43416</v>
+      </c>
+      <c r="F74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" s="2">
+        <v>43413</v>
+      </c>
+      <c r="D75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="2">
+        <v>43413</v>
+      </c>
+      <c r="D76" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="2">
+        <v>43414</v>
+      </c>
+      <c r="D77" t="s">
+        <v>69</v>
+      </c>
+      <c r="E77" s="2">
+        <v>43415</v>
+      </c>
+      <c r="F77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78" s="2">
+        <v>43414</v>
+      </c>
+      <c r="D78" t="s">
+        <v>70</v>
+      </c>
+      <c r="E78" s="2">
+        <v>43415</v>
+      </c>
+      <c r="F78" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" t="s">
+        <v>65</v>
+      </c>
+      <c r="C79" s="2">
+        <v>43414</v>
+      </c>
+      <c r="D79" t="s">
+        <v>70</v>
+      </c>
+      <c r="E79" s="2">
+        <v>43415</v>
+      </c>
+      <c r="F79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="2">
+        <v>43414</v>
+      </c>
+      <c r="D80" t="s">
+        <v>70</v>
+      </c>
+      <c r="E80" s="2">
+        <v>43415</v>
+      </c>
+      <c r="F80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" t="s">
+        <v>63</v>
+      </c>
+      <c r="C81" s="2">
+        <v>43419</v>
+      </c>
+      <c r="D81" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="2">
+        <v>43420</v>
+      </c>
+      <c r="F81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" s="2">
+        <v>43419</v>
+      </c>
+      <c r="D82" t="s">
+        <v>70</v>
+      </c>
+      <c r="E82" s="2">
+        <v>43435</v>
+      </c>
+      <c r="F82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="2">
+        <v>43419</v>
+      </c>
+      <c r="D83" t="s">
+        <v>69</v>
+      </c>
+      <c r="E83" s="2">
+        <v>43435</v>
+      </c>
+      <c r="F83" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="2">
+        <v>43420</v>
+      </c>
+      <c r="D84" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" s="2">
+        <v>43429</v>
+      </c>
+      <c r="D85" t="s">
+        <v>69</v>
+      </c>
+      <c r="E85" s="2">
+        <v>43433</v>
+      </c>
+      <c r="F85" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" t="s">
+        <v>61</v>
+      </c>
+      <c r="C86" s="2">
+        <v>43434</v>
+      </c>
+      <c r="D86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" t="s">
+        <v>63</v>
+      </c>
+      <c r="C87" s="2">
+        <v>43446</v>
+      </c>
+      <c r="D87" t="s">
+        <v>69</v>
+      </c>
+      <c r="E87" s="2">
+        <v>43446</v>
+      </c>
+      <c r="F87" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B88" t="s">
+        <v>65</v>
+      </c>
+      <c r="C88" s="2">
+        <v>43446</v>
+      </c>
+      <c r="D88" t="s">
+        <v>69</v>
+      </c>
+      <c r="E88" t="s">
+        <v>84</v>
+      </c>
+      <c r="F88" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding to work excel
</commit_message>
<xml_diff>
--- a/doc/Work.xlsx
+++ b/doc/Work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\desktop\Final Year\SoftwareEng\caffeine\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Mannion\Google Drive\Stage 5\Software Engineering\Project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F4C837-53A0-4CEC-9FF4-7F130913288C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C5AEC-9311-454F-BC6D-62BF208B05F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="28800" windowHeight="12756" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="169">
   <si>
     <t>Item</t>
   </si>
@@ -529,6 +529,15 @@
   </si>
   <si>
     <t>Spin procedure not being followed correctly</t>
+  </si>
+  <si>
+    <t>Refactoring of CardDecks to remove redundant abstract base class, generify deck</t>
+  </si>
+  <si>
+    <t>Refactor</t>
+  </si>
+  <si>
+    <t>Completed, unit and integration tests all passing</t>
   </si>
 </sst>
 </file>
@@ -885,24 +894,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021C5E94-141C-4B62-B501-75972CDFF5D4}">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -942,7 +951,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
@@ -962,7 +971,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
@@ -982,7 +991,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>119</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>120</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>125</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>126</v>
       </c>
@@ -1119,7 +1128,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>127</v>
       </c>
@@ -1139,7 +1148,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>129</v>
       </c>
@@ -1159,7 +1168,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>131</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>132</v>
       </c>
@@ -1219,7 +1228,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>133</v>
       </c>
@@ -1239,7 +1248,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>134</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>135</v>
       </c>
@@ -1279,7 +1288,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -1299,7 +1308,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>137</v>
       </c>
@@ -1319,7 +1328,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>139</v>
       </c>
@@ -1339,7 +1348,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>141</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>143</v>
       </c>
@@ -1379,7 +1388,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>145</v>
       </c>
@@ -1399,7 +1408,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>147</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>149</v>
       </c>
@@ -1439,7 +1448,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>151</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>153</v>
       </c>
@@ -1479,7 +1488,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>155</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>157</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1539,7 +1548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>158</v>
       </c>
@@ -1554,7 +1563,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>159</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1674,7 +1683,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1703,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1709,7 +1718,7 @@
       </c>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -1729,7 +1738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -1749,7 +1758,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>81</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1789,7 +1798,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1809,7 +1818,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -1829,7 +1838,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1849,7 +1858,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1869,7 +1878,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1889,7 +1898,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -1929,7 +1938,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -1949,7 +1958,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -1969,7 +1978,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -1989,7 +1998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>15</v>
       </c>
@@ -2009,7 +2018,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
@@ -2029,7 +2038,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
@@ -2067,7 +2076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>19</v>
       </c>
@@ -2087,7 +2096,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
@@ -2107,7 +2116,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -2127,7 +2136,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>22</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>53</v>
       </c>
@@ -2167,7 +2176,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>51</v>
       </c>
@@ -2187,7 +2196,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>50</v>
       </c>
@@ -2207,7 +2216,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>23</v>
       </c>
@@ -2227,7 +2236,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>49</v>
       </c>
@@ -2247,7 +2256,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -2267,7 +2276,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
@@ -2307,7 +2316,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>26</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>27</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -2381,7 +2390,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>106</v>
       </c>
@@ -2415,7 +2424,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>31</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>32</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -2475,7 +2484,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -2495,7 +2504,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -2535,7 +2544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -2549,7 +2558,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>38</v>
       </c>
@@ -2569,7 +2578,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -2584,7 +2593,7 @@
       </c>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>68</v>
       </c>
@@ -2604,7 +2613,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -2624,7 +2633,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>162</v>
       </c>
@@ -2644,7 +2653,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>164</v>
       </c>
@@ -2662,6 +2671,26 @@
       </c>
       <c r="F90" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" s="2">
+        <v>43449</v>
+      </c>
+      <c r="D91" t="s">
+        <v>73</v>
+      </c>
+      <c r="E91" s="2">
+        <v>43449</v>
+      </c>
+      <c r="F91" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slight modifications to designdoc
</commit_message>
<xml_diff>
--- a/doc/Work.xlsx
+++ b/doc/Work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Mannion\Google Drive\Stage 5\Software Engineering\Project\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\desktop\Final Year\SoftwareEng\caffeine\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C5AEC-9311-454F-BC6D-62BF208B05F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBAB178-7438-4B80-8D9D-9CC306EB01CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="28800" windowHeight="12756" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -896,22 +896,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021C5E94-141C-4B62-B501-75972CDFF5D4}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -951,7 +951,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
@@ -971,7 +971,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
@@ -991,7 +991,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>119</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>120</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>125</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>126</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>127</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>129</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>131</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>132</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>133</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>134</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>135</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>137</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>139</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>141</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>143</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>145</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>147</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>149</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>151</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>153</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>155</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>157</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>158</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>159</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>81</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>15</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>19</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>22</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>53</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>51</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>50</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>23</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>49</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>26</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>27</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>106</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>31</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>32</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>38</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="E86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>68</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>162</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>164</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Add work at end
</commit_message>
<xml_diff>
--- a/doc/Work.xlsx
+++ b/doc/Work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Mannion\Google Drive\Stage 5\Software Engineering\Project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C5AEC-9311-454F-BC6D-62BF208B05F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C012022D-AF84-4223-8505-9FFFFF663789}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="28800" windowHeight="12756" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="28800" windowHeight="12756" xr2:uid="{297F796B-6BA3-40D0-AA38-C1AB15842822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="172">
   <si>
     <t>Item</t>
   </si>
@@ -519,9 +519,6 @@
     <t>Was actually already done.</t>
   </si>
   <si>
-    <t>CareerChange pompts a player with a CollegeCareer with StandardCareer options</t>
-  </si>
-  <si>
     <t>Fixed, career type was not being set correctly</t>
   </si>
   <si>
@@ -538,6 +535,18 @@
   </si>
   <si>
     <t>Completed, unit and integration tests all passing</t>
+  </si>
+  <si>
+    <t>Refactoring of GameBoard initialisation to use façade design pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java utility classes in separate project to manipulate the game board tile positions, scaling in JSON </t>
+  </si>
+  <si>
+    <t>Board displays correctly in UI</t>
+  </si>
+  <si>
+    <t>CareerChange prompts a player with a CollegeCareer with StandardCareer options</t>
   </si>
 </sst>
 </file>
@@ -894,11 +903,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021C5E94-141C-4B62-B501-75972CDFF5D4}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2635,62 +2644,102 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C89" s="2">
+        <v>43446</v>
+      </c>
+      <c r="D89" t="s">
+        <v>73</v>
+      </c>
+      <c r="E89" s="2">
         <v>43447</v>
       </c>
-      <c r="D89" t="s">
-        <v>73</v>
-      </c>
-      <c r="E89" s="2">
-        <v>43448</v>
-      </c>
       <c r="F89" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B90" t="s">
         <v>61</v>
       </c>
       <c r="C90" s="2">
-        <v>43449</v>
+        <v>43447</v>
       </c>
       <c r="D90" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E90" s="2">
-        <v>43450</v>
+        <v>43448</v>
       </c>
       <c r="F90" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>167</v>
+        <v>61</v>
       </c>
       <c r="C91" s="2">
         <v>43449</v>
       </c>
       <c r="D91" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E91" s="2">
+        <v>43450</v>
+      </c>
+      <c r="F91" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>165</v>
+      </c>
+      <c r="B92" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" s="2">
         <v>43449</v>
       </c>
-      <c r="F91" t="s">
+      <c r="D92" t="s">
+        <v>73</v>
+      </c>
+      <c r="E92" s="2">
+        <v>43449</v>
+      </c>
+      <c r="F92" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>168</v>
+      </c>
+      <c r="B93" t="s">
+        <v>166</v>
+      </c>
+      <c r="C93" s="2">
+        <v>43453</v>
+      </c>
+      <c r="D93" t="s">
+        <v>73</v>
+      </c>
+      <c r="E93" s="2">
+        <v>43453</v>
+      </c>
+      <c r="F93" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>